<commit_message>
make no-gov items assessable and add an IG for them
</commit_message>
<xml_diff>
--- a/tools/excel/bio2/bio2.xlsx
+++ b/tools/excel/bio2/bio2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/bio2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1416A1-67BA-4540-B6F7-23B4165A2669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8F03E5-BBEC-E048-B693-36601846CFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-28200" windowWidth="51200" windowHeight="26940" xr2:uid="{51E6D8A9-FAFD-2543-B5A1-6F8F7A044C9B}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20440" activeTab="2" xr2:uid="{51E6D8A9-FAFD-2543-B5A1-6F8F7A044C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="456">
   <si>
     <t>5.01.01</t>
   </si>
@@ -1565,6 +1565,27 @@
   <si>
     <t>Baseline Informatiebeveiliging Overheid 2 (BIO2)
 24 september 2025, versie 1.2 definitief</t>
+  </si>
+  <si>
+    <t>Overheidsrisico,no_gov</t>
+  </si>
+  <si>
+    <t>Basishygiëne, ketenhygiëne,no_gov</t>
+  </si>
+  <si>
+    <t>Ketenhygiëne,no_gov</t>
+  </si>
+  <si>
+    <t>Basishygiëne,no_gov</t>
+  </si>
+  <si>
+    <t>no_gov</t>
+  </si>
+  <si>
+    <t>Geen overheidsmaatregel</t>
+  </si>
+  <si>
+    <t>No Government risk</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1717,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="2" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2040,7 +2061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CC694E-847F-1646-8DAD-3E124FC39483}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+    <sheetView zoomScale="158" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2255,17 +2276,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1180AF3C-BAFA-FF44-AD88-AAE5B9859B26}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="132" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
     <col min="5" max="5" width="94" customWidth="1"/>
     <col min="6" max="6" width="201.83203125" customWidth="1"/>
   </cols>
@@ -2290,7 +2312,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="195" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>299</v>
       </c>
@@ -2310,7 +2332,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>299</v>
       </c>
@@ -2330,7 +2352,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="65" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="65" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -2350,7 +2372,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -2371,6 +2393,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>299</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
@@ -2378,7 +2403,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -2387,7 +2412,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>299</v>
       </c>
@@ -2407,7 +2432,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>299</v>
       </c>
@@ -2427,7 +2452,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -2447,7 +2472,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>299</v>
       </c>
@@ -2468,6 +2493,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>299</v>
+      </c>
       <c r="B11">
         <v>1</v>
       </c>
@@ -2475,7 +2503,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -2484,7 +2512,10 @@
         <v>320</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>299</v>
+      </c>
       <c r="B12">
         <v>1</v>
       </c>
@@ -2492,7 +2523,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>2</v>
+        <v>450</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
@@ -2501,7 +2532,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>299</v>
       </c>
@@ -2521,7 +2552,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="78" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="78" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>299</v>
       </c>
@@ -2542,6 +2573,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>299</v>
+      </c>
       <c r="B15">
         <v>1</v>
       </c>
@@ -2559,6 +2593,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>299</v>
+      </c>
       <c r="B16">
         <v>1</v>
       </c>
@@ -2566,7 +2603,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -2575,7 +2612,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>299</v>
       </c>
@@ -2596,6 +2633,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>299</v>
+      </c>
       <c r="B18">
         <v>1</v>
       </c>
@@ -2603,7 +2643,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>21</v>
+        <v>451</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
@@ -2612,7 +2652,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="65" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="65" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>299</v>
       </c>
@@ -2632,7 +2672,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="65" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="65" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>299</v>
       </c>
@@ -2652,7 +2692,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>299</v>
       </c>
@@ -2672,7 +2712,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>299</v>
       </c>
@@ -2692,7 +2732,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>299</v>
       </c>
@@ -2712,7 +2752,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>299</v>
       </c>
@@ -2732,7 +2772,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>299</v>
       </c>
@@ -2752,7 +2792,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>299</v>
       </c>
@@ -2772,7 +2812,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="221" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="221" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>299</v>
       </c>
@@ -2792,7 +2832,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>299</v>
       </c>
@@ -2812,7 +2852,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>299</v>
       </c>
@@ -2832,7 +2872,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>299</v>
       </c>
@@ -2852,7 +2892,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>299</v>
       </c>
@@ -2872,7 +2912,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>299</v>
       </c>
@@ -2892,7 +2932,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>299</v>
       </c>
@@ -2912,7 +2952,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>299</v>
       </c>
@@ -2932,7 +2972,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="78" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="78" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>299</v>
       </c>
@@ -2952,7 +2992,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="65" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="65" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>299</v>
       </c>
@@ -2972,7 +3012,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>299</v>
       </c>
@@ -2992,7 +3032,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>299</v>
       </c>
@@ -3012,7 +3052,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -3032,7 +3072,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>299</v>
       </c>
@@ -3052,7 +3092,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>299</v>
       </c>
@@ -3072,7 +3112,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>299</v>
       </c>
@@ -3092,7 +3132,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>299</v>
       </c>
@@ -3112,7 +3152,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>299</v>
       </c>
@@ -3132,7 +3172,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="91" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="91" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>299</v>
       </c>
@@ -3152,7 +3192,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>299</v>
       </c>
@@ -3172,7 +3212,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>299</v>
       </c>
@@ -3192,7 +3232,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>299</v>
       </c>
@@ -3212,7 +3252,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>299</v>
       </c>
@@ -3232,7 +3272,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>299</v>
       </c>
@@ -3252,7 +3292,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="78" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="78" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>299</v>
       </c>
@@ -3272,7 +3312,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>299</v>
       </c>
@@ -3292,7 +3332,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>299</v>
       </c>
@@ -3313,6 +3353,9 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>299</v>
+      </c>
       <c r="B54">
         <v>1</v>
       </c>
@@ -3320,7 +3363,7 @@
         <v>104</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>11</v>
@@ -3329,7 +3372,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>299</v>
       </c>
@@ -3349,7 +3392,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>299</v>
       </c>
@@ -3369,7 +3412,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>299</v>
       </c>
@@ -3389,7 +3432,10 @@
         <v>365</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>299</v>
+      </c>
       <c r="B58">
         <v>1</v>
       </c>
@@ -3397,7 +3443,7 @@
         <v>111</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>2</v>
+        <v>450</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>11</v>
@@ -3406,7 +3452,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>299</v>
       </c>
@@ -3426,7 +3472,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>299</v>
       </c>
@@ -3446,7 +3492,10 @@
         <v>367</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>299</v>
+      </c>
       <c r="B61">
         <v>1</v>
       </c>
@@ -3454,7 +3503,7 @@
         <v>116</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>2</v>
+        <v>450</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>11</v>
@@ -3464,6 +3513,9 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>299</v>
+      </c>
       <c r="B62">
         <v>1</v>
       </c>
@@ -3471,7 +3523,7 @@
         <v>117</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>11</v>
@@ -3480,7 +3532,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>299</v>
       </c>
@@ -3501,6 +3553,9 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>299</v>
+      </c>
       <c r="B64">
         <v>1</v>
       </c>
@@ -3508,7 +3563,7 @@
         <v>120</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>11</v>
@@ -3517,7 +3572,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>299</v>
       </c>
@@ -3537,7 +3592,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>299</v>
       </c>
@@ -3557,7 +3612,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>299</v>
       </c>
@@ -3578,6 +3633,9 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>299</v>
+      </c>
       <c r="B68">
         <v>1</v>
       </c>
@@ -3585,7 +3643,7 @@
         <v>127</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>11</v>
@@ -3594,7 +3652,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>299</v>
       </c>
@@ -3614,7 +3672,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>299</v>
       </c>
@@ -3634,7 +3692,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>299</v>
       </c>
@@ -3654,7 +3712,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>299</v>
       </c>
@@ -3674,7 +3732,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>299</v>
       </c>
@@ -3695,6 +3753,9 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>299</v>
+      </c>
       <c r="B74">
         <v>1</v>
       </c>
@@ -3702,7 +3763,7 @@
         <v>138</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>11</v>
@@ -3712,14 +3773,17 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>299</v>
+      </c>
       <c r="B75">
         <v>1</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>5</v>
+      <c r="D75" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>11</v>
@@ -3729,6 +3793,9 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>299</v>
+      </c>
       <c r="B76">
         <v>1</v>
       </c>
@@ -3736,7 +3803,7 @@
         <v>140</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>11</v>
@@ -3746,14 +3813,17 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>299</v>
+      </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>5</v>
+      <c r="D77" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>11</v>
@@ -3762,7 +3832,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>299</v>
       </c>
@@ -3782,7 +3852,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>299</v>
       </c>
@@ -3802,7 +3872,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>299</v>
       </c>
@@ -3822,7 +3892,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>299</v>
       </c>
@@ -3843,6 +3913,9 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>299</v>
+      </c>
       <c r="B82">
         <v>1</v>
       </c>
@@ -3850,7 +3923,7 @@
         <v>150</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>11</v>
@@ -3860,14 +3933,17 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>299</v>
+      </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>5</v>
+      <c r="D83" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>11</v>
@@ -3877,6 +3953,9 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>299</v>
+      </c>
       <c r="B84">
         <v>1</v>
       </c>
@@ -3884,7 +3963,7 @@
         <v>152</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>11</v>
@@ -3894,14 +3973,17 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>299</v>
+      </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>5</v>
+      <c r="D85" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>11</v>
@@ -3910,7 +3992,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>299</v>
       </c>
@@ -3931,14 +4013,17 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>299</v>
+      </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>5</v>
+      <c r="D87" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>11</v>
@@ -3948,6 +4033,9 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>299</v>
+      </c>
       <c r="B88">
         <v>1</v>
       </c>
@@ -3955,7 +4043,7 @@
         <v>157</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>11</v>
@@ -3964,7 +4052,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>299</v>
       </c>
@@ -3984,7 +4072,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>299</v>
       </c>
@@ -4004,7 +4092,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>299</v>
       </c>
@@ -4025,6 +4113,9 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>299</v>
+      </c>
       <c r="B92">
         <v>1</v>
       </c>
@@ -4032,7 +4123,7 @@
         <v>164</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>11</v>
@@ -4042,14 +4133,17 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>299</v>
+      </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>5</v>
+      <c r="D93" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>11</v>
@@ -4059,6 +4153,9 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>299</v>
+      </c>
       <c r="B94">
         <v>1</v>
       </c>
@@ -4066,7 +4163,7 @@
         <v>166</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>11</v>
@@ -4076,14 +4173,17 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>299</v>
+      </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>5</v>
+      <c r="D95" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>11</v>
@@ -4092,7 +4192,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>299</v>
       </c>
@@ -4112,7 +4212,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>299</v>
       </c>
@@ -4132,7 +4232,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>299</v>
       </c>
@@ -4152,7 +4252,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -4172,7 +4272,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -4193,6 +4293,9 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>299</v>
+      </c>
       <c r="B101">
         <v>1</v>
       </c>
@@ -4200,7 +4303,7 @@
         <v>178</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>11</v>
@@ -4209,7 +4312,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>299</v>
       </c>
@@ -4230,6 +4333,9 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>299</v>
+      </c>
       <c r="B103">
         <v>1</v>
       </c>
@@ -4237,7 +4343,7 @@
         <v>181</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>11</v>
@@ -4246,7 +4352,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>299</v>
       </c>
@@ -4266,7 +4372,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>299</v>
       </c>
@@ -4286,7 +4392,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>299</v>
       </c>
@@ -4306,7 +4412,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="78" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="78" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -4326,7 +4432,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>299</v>
       </c>
@@ -4346,7 +4452,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>299</v>
       </c>
@@ -4366,7 +4472,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>299</v>
       </c>
@@ -4386,7 +4492,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" ht="52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>299</v>
       </c>
@@ -4406,7 +4512,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>299</v>
       </c>
@@ -4426,7 +4532,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" ht="52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>299</v>
       </c>
@@ -4447,14 +4553,17 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>299</v>
+      </c>
       <c r="B114">
         <v>1</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>12</v>
+      <c r="D114" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>11</v>
@@ -4464,6 +4573,9 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>299</v>
+      </c>
       <c r="B115">
         <v>1</v>
       </c>
@@ -4471,7 +4583,7 @@
         <v>203</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>11</v>
@@ -4481,14 +4593,17 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>299</v>
+      </c>
       <c r="B116">
         <v>1</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>12</v>
+      <c r="D116" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>11</v>
@@ -4498,6 +4613,9 @@
       </c>
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>299</v>
+      </c>
       <c r="B117">
         <v>1</v>
       </c>
@@ -4505,7 +4623,7 @@
         <v>205</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>11</v>
@@ -4514,7 +4632,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>299</v>
       </c>
@@ -4534,7 +4652,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>299</v>
       </c>
@@ -4554,7 +4672,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>299</v>
       </c>
@@ -4574,7 +4692,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>299</v>
       </c>
@@ -4595,14 +4713,17 @@
       </c>
     </row>
     <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>299</v>
+      </c>
       <c r="B122">
         <v>1</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>12</v>
+      <c r="D122" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>11</v>
@@ -4611,7 +4732,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>299</v>
       </c>
@@ -4631,7 +4752,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>299</v>
       </c>
@@ -4651,7 +4772,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>299</v>
       </c>
@@ -4671,7 +4792,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>299</v>
       </c>
@@ -4691,7 +4812,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>299</v>
       </c>
@@ -4711,7 +4832,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>299</v>
       </c>
@@ -4731,7 +4852,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>299</v>
       </c>
@@ -4751,7 +4872,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>299</v>
       </c>
@@ -4771,7 +4892,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>299</v>
       </c>
@@ -4791,7 +4912,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>299</v>
       </c>
@@ -4812,6 +4933,9 @@
       </c>
     </row>
     <row r="133" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>299</v>
+      </c>
       <c r="B133">
         <v>1</v>
       </c>
@@ -4819,7 +4943,7 @@
         <v>235</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>11</v>
@@ -4828,7 +4952,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>299</v>
       </c>
@@ -4848,7 +4972,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>299</v>
       </c>
@@ -4868,7 +4992,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>299</v>
       </c>
@@ -4888,7 +5012,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>299</v>
       </c>
@@ -4908,7 +5032,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>299</v>
       </c>
@@ -4928,7 +5052,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>299</v>
       </c>
@@ -4948,7 +5072,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>299</v>
       </c>
@@ -4968,7 +5092,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>299</v>
       </c>
@@ -4988,7 +5112,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>299</v>
       </c>
@@ -5008,7 +5132,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>299</v>
       </c>
@@ -5029,14 +5153,17 @@
       </c>
     </row>
     <row r="144" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>299</v>
+      </c>
       <c r="B144">
         <v>1</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D144" s="3" t="s">
-        <v>12</v>
+      <c r="D144" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>11</v>
@@ -5045,7 +5172,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>299</v>
       </c>
@@ -5065,7 +5192,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>299</v>
       </c>
@@ -5085,7 +5212,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>299</v>
       </c>
@@ -5105,7 +5232,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>299</v>
       </c>
@@ -5125,7 +5252,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>299</v>
       </c>
@@ -5146,6 +5273,9 @@
       </c>
     </row>
     <row r="150" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>299</v>
+      </c>
       <c r="B150">
         <v>1</v>
       </c>
@@ -5153,7 +5283,7 @@
         <v>267</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>11</v>
@@ -5163,6 +5293,9 @@
       </c>
     </row>
     <row r="151" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>299</v>
+      </c>
       <c r="B151">
         <v>1</v>
       </c>
@@ -5170,7 +5303,7 @@
         <v>268</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>5</v>
+        <v>452</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>11</v>
@@ -5179,7 +5312,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>299</v>
       </c>
@@ -5200,6 +5333,9 @@
       </c>
     </row>
     <row r="153" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>299</v>
+      </c>
       <c r="B153">
         <v>1</v>
       </c>
@@ -5207,7 +5343,7 @@
         <v>271</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>11</v>
@@ -5216,7 +5352,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>299</v>
       </c>
@@ -5236,7 +5372,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>299</v>
       </c>
@@ -5256,7 +5392,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>299</v>
       </c>
@@ -5276,7 +5412,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" ht="26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>299</v>
       </c>
@@ -5296,7 +5432,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>299</v>
       </c>
@@ -5316,7 +5452,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>299</v>
       </c>
@@ -5337,14 +5473,17 @@
       </c>
     </row>
     <row r="160" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>299</v>
+      </c>
       <c r="B160">
         <v>1</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D160" s="3" t="s">
-        <v>12</v>
+      <c r="D160" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>11</v>
@@ -5353,7 +5492,10 @@
         <v>320</v>
       </c>
     </row>
-    <row r="161" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>299</v>
+      </c>
       <c r="B161">
         <v>1</v>
       </c>
@@ -5361,7 +5503,7 @@
         <v>285</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>12</v>
+        <v>449</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>11</v>
@@ -5371,7 +5513,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F161" xr:uid="{1180AF3C-BAFA-FF44-AD88-AAE5B9859B26}"/>
+  <autoFilter ref="A1:F161" xr:uid="{1180AF3C-BAFA-FF44-AD88-AAE5B9859B26}">
+    <filterColumn colId="0">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5381,7 +5527,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5412,10 +5558,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C54FFF-81A2-144A-BF42-A792609CF17A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="193" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5436,7 +5582,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5467,6 +5613,17 @@
       </c>
       <c r="C4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C5" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve naming / align framework naming to library
</commit_message>
<xml_diff>
--- a/tools/excel/bio2/bio2.xlsx
+++ b/tools/excel/bio2/bio2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/bio2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FF262-DEA9-AC47-A145-B7B95119CB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE57CBB3-D588-404B-B0CE-DD3F6A702B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20440" activeTab="4" xr2:uid="{51E6D8A9-FAFD-2543-B5A1-6F8F7A044C9B}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20440" activeTab="1" xr2:uid="{51E6D8A9-FAFD-2543-B5A1-6F8F7A044C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="404">
   <si>
     <t>5.01.01</t>
   </si>
@@ -913,9 +913,6 @@
     <t>urn:intuitem:risk:framework:bio2</t>
   </si>
   <si>
-    <t>BIO2</t>
-  </si>
-  <si>
     <t>bio2</t>
   </si>
   <si>
@@ -947,12 +944,6 @@
   </si>
   <si>
     <t>intuitem</t>
-  </si>
-  <si>
-    <t>name[en]</t>
-  </si>
-  <si>
-    <t>description[en]</t>
   </si>
   <si>
     <t>Baseline Information Security for Government 2 (BIO2)</t>
@@ -1433,12 +1424,14 @@
     <t>The Baseline Information Security for Government 2 (BIO2) is entirely structured in accordance with NEN-EN-ISO/IEC 27001, Annex A and NEN-EN-ISO/IEC 27002. The Netherlands Standardisation Forum has included these standards in the ‘comply-or-explain’ list with compulsory standards for the public sector, in accordance with the comply-or-explain principle. This means that the government will apply these standards unless there are explicitly formulated reasons not to do so. The BIO2 describes the concrete details of the latest version of NEN-EN-ISO/IEC 27001 and NEN-EN-ISO/IEC 27002 for the government. It does not replace these two standards. The BIO2 only includes specific government measures. NEN-EN-ISO/IEC 27001 and NEN-EN-ISO/IEC 27002 describe the details for implementation (guidelines) and requirements for process structure (the ISMS from NEN-EN-ISO/IEC 27001). The structure of the management system for information security must comply with ISO 27001. Where the BIO2 does not specifically prescribe certain rules, both ISO documents must be used to ensure a solid risk management structure. The ISO documents therefore provide the application details that are not described in the BIO2 but which are nevertheless necessary for its proper implementation. The use of NEN-EN-ISO/IEC standards 27001 and 27002 in the BIO is copyright protected. The use of texts from these standards in the BIO is subject to permission by the Netherlands Standardization Institute. For more information about NEN and the use of their products, see: www.nen.nl.</t>
   </si>
   <si>
+    <t>Baseline Informatiebeveiliging Overheid 2 (BIO2)
+24 september 2025, versie 1.2 definitief
+De BIO2 is de opvolger van de BIO 1.04zv. Het is de vernieuwde basisnorm voor informatiebeveiliging binnen de Nederlandse overheid. De BIO2 biedt een uniforme aanpak en een gemeenschappelijk normenkader voor informatiebeveiliging binnen de overheid, waarbij risicomanagement centraal staat.</t>
+  </si>
+  <si>
     <t>Baseline Information Security for Government 2 (BIO2)
-24 September 2025, version 1.2 final</t>
-  </si>
-  <si>
-    <t>Baseline Informatiebeveiliging Overheid 2 (BIO2)
-24 september 2025, versie 1.2 definitief</t>
+24 September 2025, version 1.2 final
+The BIO2 is the successor of the BIO 1.04zv. It is the renewed basic standard for information security within the Dutch government. The BIO2 offers a uniform approach and a common framework of standards for information security within the government, in which risk management is central.</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1526,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1557,7 +1550,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1914,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CC694E-847F-1646-8DAD-3E124FC39483}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1929,7 +1921,7 @@
         <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1937,12 +1929,12 @@
         <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1950,10 +1942,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1961,47 +1953,47 @@
         <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>393</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2009,23 +2001,23 @@
         <v>249</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>405</v>
+      <c r="B12" s="14" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -2037,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81D0AEB-8843-7C4B-B71A-E03B6E4AD5FA}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2068,23 +2060,23 @@
         <v>245</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>249</v>
       </c>
-      <c r="B4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>250</v>
       </c>
-      <c r="B5" t="s">
-        <v>262</v>
+      <c r="B5" s="14" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2092,7 +2084,7 @@
         <v>251</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2105,18 +2097,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+      <c r="B8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>274</v>
+        <v>392</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2158,30 +2150,30 @@
         <v>254</v>
       </c>
       <c r="E1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="195" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="195" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>275</v>
+      <c r="E2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2200,8 +2192,8 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>276</v>
+      <c r="F3" s="12" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="65" x14ac:dyDescent="0.2">
@@ -2221,7 +2213,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2240,8 +2232,8 @@
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>278</v>
+      <c r="F5" s="12" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="52" x14ac:dyDescent="0.2">
@@ -2261,7 +2253,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2281,7 +2273,7 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2301,7 +2293,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2321,7 +2313,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2340,8 +2332,8 @@
       <c r="E10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>283</v>
+      <c r="F10" s="12" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="78" x14ac:dyDescent="0.2">
@@ -2361,7 +2353,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2381,7 +2373,7 @@
         <v>25</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="65" x14ac:dyDescent="0.2">
@@ -2401,7 +2393,7 @@
         <v>27</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="65" x14ac:dyDescent="0.2">
@@ -2421,7 +2413,7 @@
         <v>29</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2441,7 +2433,7 @@
         <v>31</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2461,7 +2453,7 @@
         <v>33</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2481,7 +2473,7 @@
         <v>35</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -2501,7 +2493,7 @@
         <v>37</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2521,7 +2513,7 @@
         <v>39</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2541,7 +2533,7 @@
         <v>41</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="221" x14ac:dyDescent="0.2">
@@ -2561,7 +2553,7 @@
         <v>43</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2581,7 +2573,7 @@
         <v>45</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2601,7 +2593,7 @@
         <v>47</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2621,7 +2613,7 @@
         <v>49</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2641,7 +2633,7 @@
         <v>51</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2661,7 +2653,7 @@
         <v>53</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2681,7 +2673,7 @@
         <v>55</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="52" x14ac:dyDescent="0.2">
@@ -2701,7 +2693,7 @@
         <v>57</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="78" x14ac:dyDescent="0.2">
@@ -2721,7 +2713,7 @@
         <v>59</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="65" x14ac:dyDescent="0.2">
@@ -2741,7 +2733,7 @@
         <v>61</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2761,7 +2753,7 @@
         <v>63</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2781,7 +2773,7 @@
         <v>65</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2801,7 +2793,7 @@
         <v>67</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2821,7 +2813,7 @@
         <v>69</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2841,7 +2833,7 @@
         <v>71</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -2861,7 +2853,7 @@
         <v>73</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="52" x14ac:dyDescent="0.2">
@@ -2881,7 +2873,7 @@
         <v>75</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2901,7 +2893,7 @@
         <v>77</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="91" x14ac:dyDescent="0.2">
@@ -2921,7 +2913,7 @@
         <v>79</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -2941,7 +2933,7 @@
         <v>81</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2961,7 +2953,7 @@
         <v>83</v>
       </c>
       <c r="F41" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2981,7 +2973,7 @@
         <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3001,7 +2993,7 @@
         <v>87</v>
       </c>
       <c r="F43" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -3021,7 +3013,7 @@
         <v>89</v>
       </c>
       <c r="F44" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="78" x14ac:dyDescent="0.2">
@@ -3041,7 +3033,7 @@
         <v>91</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3061,7 +3053,7 @@
         <v>93</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -3081,7 +3073,7 @@
         <v>95</v>
       </c>
       <c r="F47" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3101,7 +3093,7 @@
         <v>98</v>
       </c>
       <c r="F48" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3121,7 +3113,7 @@
         <v>100</v>
       </c>
       <c r="F49" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -3141,7 +3133,7 @@
         <v>102</v>
       </c>
       <c r="F50" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3161,7 +3153,7 @@
         <v>104</v>
       </c>
       <c r="F51" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3181,7 +3173,7 @@
         <v>106</v>
       </c>
       <c r="F52" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3201,7 +3193,7 @@
         <v>108</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -3221,7 +3213,7 @@
         <v>110</v>
       </c>
       <c r="F54" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3241,7 +3233,7 @@
         <v>112</v>
       </c>
       <c r="F55" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="52" x14ac:dyDescent="0.2">
@@ -3261,7 +3253,7 @@
         <v>114</v>
       </c>
       <c r="F56" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3281,7 +3273,7 @@
         <v>116</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -3301,7 +3293,7 @@
         <v>118</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -3321,7 +3313,7 @@
         <v>120</v>
       </c>
       <c r="F59" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3341,7 +3333,7 @@
         <v>122</v>
       </c>
       <c r="F60" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -3361,7 +3353,7 @@
         <v>124</v>
       </c>
       <c r="F61" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3381,7 +3373,7 @@
         <v>126</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -3401,7 +3393,7 @@
         <v>128</v>
       </c>
       <c r="F63" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3421,7 +3413,7 @@
         <v>130</v>
       </c>
       <c r="F64" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3441,7 +3433,7 @@
         <v>132</v>
       </c>
       <c r="F65" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3460,8 +3452,8 @@
       <c r="E66" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F66" s="14" t="s">
-        <v>339</v>
+      <c r="F66" s="13" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3481,7 +3473,7 @@
         <v>136</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -3501,7 +3493,7 @@
         <v>138</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3521,7 +3513,7 @@
         <v>140</v>
       </c>
       <c r="F69" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -3541,7 +3533,7 @@
         <v>142</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="119" x14ac:dyDescent="0.2">
@@ -3561,7 +3553,7 @@
         <v>144</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3581,7 +3573,7 @@
         <v>146</v>
       </c>
       <c r="F72" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -3601,7 +3593,7 @@
         <v>148</v>
       </c>
       <c r="F73" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3621,7 +3613,7 @@
         <v>150</v>
       </c>
       <c r="F74" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3641,7 +3633,7 @@
         <v>152</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3661,7 +3653,7 @@
         <v>154</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3681,7 +3673,7 @@
         <v>156</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3701,7 +3693,7 @@
         <v>158</v>
       </c>
       <c r="F78" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="78" x14ac:dyDescent="0.2">
@@ -3721,7 +3713,7 @@
         <v>160</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3741,7 +3733,7 @@
         <v>162</v>
       </c>
       <c r="F80" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -3761,7 +3753,7 @@
         <v>164</v>
       </c>
       <c r="F81" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3781,7 +3773,7 @@
         <v>166</v>
       </c>
       <c r="F82" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="52" x14ac:dyDescent="0.2">
@@ -3801,7 +3793,7 @@
         <v>168</v>
       </c>
       <c r="F83" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -3821,7 +3813,7 @@
         <v>170</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="52" x14ac:dyDescent="0.2">
@@ -3841,7 +3833,7 @@
         <v>172</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3861,7 +3853,7 @@
         <v>174</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3881,7 +3873,7 @@
         <v>176</v>
       </c>
       <c r="F87" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3901,7 +3893,7 @@
         <v>178</v>
       </c>
       <c r="F88" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -3921,7 +3913,7 @@
         <v>180</v>
       </c>
       <c r="F89" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="119" x14ac:dyDescent="0.2">
@@ -3941,7 +3933,7 @@
         <v>182</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3961,7 +3953,7 @@
         <v>184</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3981,7 +3973,7 @@
         <v>186</v>
       </c>
       <c r="F92" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4001,7 +3993,7 @@
         <v>188</v>
       </c>
       <c r="F93" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4021,7 +4013,7 @@
         <v>190</v>
       </c>
       <c r="F94" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4041,7 +4033,7 @@
         <v>192</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4061,7 +4053,7 @@
         <v>194</v>
       </c>
       <c r="F96" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4081,7 +4073,7 @@
         <v>196</v>
       </c>
       <c r="F97" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4101,7 +4093,7 @@
         <v>198</v>
       </c>
       <c r="F98" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4121,7 +4113,7 @@
         <v>200</v>
       </c>
       <c r="F99" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4141,7 +4133,7 @@
         <v>202</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4161,7 +4153,7 @@
         <v>204</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4181,7 +4173,7 @@
         <v>206</v>
       </c>
       <c r="F102" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4201,7 +4193,7 @@
         <v>208</v>
       </c>
       <c r="F103" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4221,7 +4213,7 @@
         <v>210</v>
       </c>
       <c r="F104" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="39" x14ac:dyDescent="0.2">
@@ -4241,7 +4233,7 @@
         <v>212</v>
       </c>
       <c r="F105" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4261,7 +4253,7 @@
         <v>214</v>
       </c>
       <c r="F106" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4281,7 +4273,7 @@
         <v>216</v>
       </c>
       <c r="F107" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -4301,7 +4293,7 @@
         <v>218</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -4320,8 +4312,8 @@
       <c r="E109" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F109" s="13" t="s">
-        <v>381</v>
+      <c r="F109" s="12" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -4341,7 +4333,7 @@
         <v>222</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4361,7 +4353,7 @@
         <v>224</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -4381,7 +4373,7 @@
         <v>226</v>
       </c>
       <c r="F112" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4401,7 +4393,7 @@
         <v>228</v>
       </c>
       <c r="F113" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4421,7 +4413,7 @@
         <v>230</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4441,7 +4433,7 @@
         <v>232</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4461,7 +4453,7 @@
         <v>234</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4481,7 +4473,7 @@
         <v>236</v>
       </c>
       <c r="F117" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4501,7 +4493,7 @@
         <v>238</v>
       </c>
       <c r="F118" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="26" x14ac:dyDescent="0.2">
@@ -4521,7 +4513,7 @@
         <v>240</v>
       </c>
       <c r="F119" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4541,7 +4533,7 @@
         <v>242</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -4561,7 +4553,7 @@
         <v>244</v>
       </c>
       <c r="F121" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -4608,7 +4600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C54FFF-81A2-144A-BF42-A792609CF17A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" workbookViewId="0">
+    <sheetView zoomScale="193" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -4627,7 +4619,7 @@
         <v>249</v>
       </c>
       <c r="C1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -4635,7 +4627,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -4646,7 +4638,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C3" t="s">
         <v>255</v>
@@ -4657,7 +4649,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>

</xml_diff>